<commit_message>
feat: add get transaction date func
</commit_message>
<xml_diff>
--- a/scripts/samples.xlsx
+++ b/scripts/samples.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
   <si>
     <t>name</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>balanceOutstanding</t>
+  </si>
+  <si>
+    <t>transactionDate</t>
   </si>
   <si>
     <t>Account debit</t>
@@ -78,6 +81,9 @@
     <t>68896.30</t>
   </si>
   <si>
+    <t>2023-01-05 00:00:00.000Z</t>
+  </si>
+  <si>
     <t>Account Credit - Canara Bank</t>
   </si>
   <si>
@@ -96,6 +102,9 @@
     <t>35763.88</t>
   </si>
   <si>
+    <t>2022-12-30 00:00:00.000Z</t>
+  </si>
+  <si>
     <t>Account Credit - KBL Bank</t>
   </si>
   <si>
@@ -108,6 +117,9 @@
     <t>6635.00</t>
   </si>
   <si>
+    <t>2022-12-21 00:00:00.000Z</t>
+  </si>
+  <si>
     <t>Account Debit - Karnataka Bank</t>
   </si>
   <si>
@@ -115,6 +127,9 @@
   </si>
   <si>
     <t>40.00</t>
+  </si>
+  <si>
+    <t>2022-12-23 00:00:00.000Z</t>
   </si>
   <si>
     <t>Account Credit - NEFT/PAYPAL</t>
@@ -127,6 +142,9 @@
   </si>
   <si>
     <t>120791.02</t>
+  </si>
+  <si>
+    <t>2022-11-30 00:00:00.000Z</t>
   </si>
   <si>
     <t>Account Credited - NEFT/OITO LABS</t>
@@ -198,13 +216,13 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -469,162 +487,183 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="F2" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" s="2">
         <v>2343.23</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>16</v>
+      <c r="H3" s="8" t="s">
+        <v>20</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>11</v>
+      <c r="J3" s="3" t="s">
+        <v>21</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>17</v>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>22</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="J5" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="J6" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>14</v>
+      <c r="F7" s="5" t="s">
+        <v>40</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>27</v>
+      <c r="H7" s="5" t="s">
+        <v>41</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
+      <c r="J7" s="3" t="s">
+        <v>42</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>28</v>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>43</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>29</v>
+      <c r="B8" s="3" t="s">
+        <v>44</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>11</v>
+      <c r="C8" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>39</v>
+      <c r="F8" s="5" t="s">
+        <v>45</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>24</v>
+      <c r="G8" s="4" t="s">
+        <v>26</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>40</v>
+      <c r="H8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
feat: add getBankName function
</commit_message>
<xml_diff>
--- a/scripts/samples.xlsx
+++ b/scripts/samples.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhLBCrkEqqC+VKHVntlqaL3v9bbfg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7miBACPygJQx2GV73t1R3Uh81PIqPA=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
   <si>
     <t>name</t>
   </si>
@@ -48,6 +48,9 @@
     <t>transactionDate</t>
   </si>
   <si>
+    <t>bankName</t>
+  </si>
+  <si>
     <t>Account debit</t>
   </si>
   <si>
@@ -66,6 +69,9 @@
     <t>debit</t>
   </si>
   <si>
+    <t>BNF</t>
+  </si>
+  <si>
     <t>Account debit - UNION-Bank</t>
   </si>
   <si>
@@ -82,6 +88,9 @@
   </si>
   <si>
     <t>2023-01-05 00:00:00.000Z</t>
+  </si>
+  <si>
+    <t>Union Bank of India</t>
   </si>
   <si>
     <t>Account Credit - Canara Bank</t>
@@ -105,6 +114,9 @@
     <t>2022-12-30 00:00:00.000Z</t>
   </si>
   <si>
+    <t>Canara Bank</t>
+  </si>
+  <si>
     <t>Account Credit - KBL Bank</t>
   </si>
   <si>
@@ -120,6 +132,9 @@
     <t>2022-12-21 00:00:00.000Z</t>
   </si>
   <si>
+    <t>KBL</t>
+  </si>
+  <si>
     <t>Account Debit - Karnataka Bank</t>
   </si>
   <si>
@@ -130,6 +145,9 @@
   </si>
   <si>
     <t>2022-12-23 00:00:00.000Z</t>
+  </si>
+  <si>
+    <t>Karnataka Bank</t>
   </si>
   <si>
     <t>Account Credit - NEFT/PAYPAL</t>
@@ -490,180 +508,204 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" s="2">
         <v>2343.23</v>
       </c>
+      <c r="K2" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="H3" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H5" s="2"/>
       <c r="J5" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>31</v>
-      </c>
       <c r="F6" s="5" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H6" s="2"/>
       <c r="J6" s="3" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>42</v>
+        <v>48</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">

</xml_diff>